<commit_message>
Any file with Ra_Stock_5 used had the wrong concentration for stock 5 radium, this was adjusted.
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaGoe_pH9/RaGoe_pH9_NoScript.xlsx
+++ b/Sorption Experiments/RaGoe_pH9/RaGoe_pH9_NoScript.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="12285" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -823,11 +823,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="510836048"/>
-        <c:axId val="510833696"/>
+        <c:axId val="154991208"/>
+        <c:axId val="148491136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="510836048"/>
+        <c:axId val="154991208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,12 +855,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="510833696"/>
+        <c:crossAx val="148491136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="510833696"/>
+        <c:axId val="148491136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -888,7 +888,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="510836048"/>
+        <c:crossAx val="154991208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1211,7 +1211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
@@ -1284,10 +1284,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>675.45997631774435</v>
-      </c>
-      <c r="C6">
-        <v>0.13742948708443162</v>
+        <v>1407</v>
+      </c>
+      <c r="C6" s="17">
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -6489,7 +6489,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
+      <selection pane="bottomRight" activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6848,19 +6848,19 @@
       </c>
       <c r="S5">
         <f>B5*Parameters!$B$6</f>
-        <v>4.6944468354083231</v>
+        <v>9.778649999999999</v>
       </c>
       <c r="T5">
         <f>SQRT((C5/B5)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S5</f>
-        <v>6.8217960029032382E-3</v>
+        <v>0.43112964975747142</v>
       </c>
       <c r="U5">
         <f t="shared" si="4"/>
-        <v>102.82536548011423</v>
+        <v>267.36268472256324</v>
       </c>
       <c r="W5">
         <f t="shared" si="5"/>
-        <v>0.67682176510561509</v>
+        <v>0.84485148337727656</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -6916,19 +6916,19 @@
       </c>
       <c r="S6">
         <f>B6*Parameters!$B$6</f>
-        <v>4.6944468354083231</v>
+        <v>9.778649999999999</v>
       </c>
       <c r="T6">
         <f>SQRT((C6/B6)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S6</f>
-        <v>6.8217960029032382E-3</v>
+        <v>0.43112964975747142</v>
       </c>
       <c r="U6">
         <f t="shared" si="4"/>
-        <v>104.36334024201831</v>
+        <v>274.40357986046905</v>
       </c>
       <c r="W6">
         <f t="shared" si="5"/>
-        <v>0.66471385929859594</v>
+        <v>0.83903882824602827</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -6984,19 +6984,19 @@
       </c>
       <c r="S7">
         <f>B7*Parameters!$B$6</f>
-        <v>4.6944468354083231</v>
+        <v>9.778649999999999</v>
       </c>
       <c r="T7">
         <f>SQRT((C7/B7)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S7</f>
-        <v>6.8217960029032382E-3</v>
+        <v>0.43112964975747142</v>
       </c>
       <c r="U7">
         <f t="shared" si="4"/>
-        <v>103.43887812319161</v>
+        <v>270.68240327423359</v>
       </c>
       <c r="W7">
         <f t="shared" si="5"/>
-        <v>0.66984290273073521</v>
+        <v>0.8415011335446817</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7052,19 +7052,19 @@
       </c>
       <c r="S8">
         <f>B8*Parameters!$B$6</f>
-        <v>23.506007175857501</v>
+        <v>48.9636</v>
       </c>
       <c r="T8">
         <f>SQRT((C8/B8)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S8</f>
-        <v>6.7715098344118985E-2</v>
+        <v>2.1621827512955516</v>
       </c>
       <c r="U8">
         <f t="shared" si="4"/>
-        <v>683.46331863284558</v>
+        <v>1512.7008699078453</v>
       </c>
       <c r="W8">
         <f t="shared" si="5"/>
-        <v>0.89263666623818783</v>
+        <v>0.94845797094516859</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -7120,19 +7120,19 @@
       </c>
       <c r="S9">
         <f>B9*Parameters!$B$6</f>
-        <v>23.506007175857501</v>
+        <v>48.9636</v>
       </c>
       <c r="T9">
         <f>SQRT((C9/B9)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S9</f>
-        <v>6.7715098344118985E-2</v>
+        <v>2.1621827512955516</v>
       </c>
       <c r="U9">
         <f t="shared" si="4"/>
-        <v>692.22491353835881</v>
+        <v>1555.1941618143758</v>
       </c>
       <c r="W9">
         <f t="shared" si="5"/>
-        <v>0.86874111781754093</v>
+        <v>0.93698640977224068</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -7188,19 +7188,19 @@
       </c>
       <c r="S10">
         <f>B10*Parameters!$B$6</f>
-        <v>23.506007175857501</v>
+        <v>48.9636</v>
       </c>
       <c r="T10">
         <f>SQRT((C10/B10)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S10</f>
-        <v>6.7715098344118985E-2</v>
+        <v>2.1621827512955516</v>
       </c>
       <c r="U10">
         <f t="shared" si="4"/>
-        <v>703.83492612957286</v>
+        <v>1563.8887377560086</v>
       </c>
       <c r="W10">
         <f t="shared" si="5"/>
-        <v>0.88630594118226069</v>
+        <v>0.94541877307995847</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -7256,19 +7256,19 @@
       </c>
       <c r="S11">
         <f>B11*Parameters!$B$6</f>
-        <v>46.944468354083234</v>
+        <v>97.786500000000004</v>
       </c>
       <c r="T11">
         <f>SQRT((C11/B11)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S11</f>
-        <v>6.8217960029032368E-2</v>
+        <v>4.3112964975747143</v>
       </c>
       <c r="U11">
         <f t="shared" si="4"/>
-        <v>1302.8808877324973</v>
+        <v>2980.8357275317303</v>
       </c>
       <c r="W11">
         <f t="shared" si="5"/>
-        <v>0.84093594586125353</v>
+        <v>0.92363795149853434</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -7324,19 +7324,19 @@
       </c>
       <c r="S12">
         <f>B12*Parameters!$B$6</f>
-        <v>46.944468354083234</v>
+        <v>97.786500000000004</v>
       </c>
       <c r="T12">
         <f>SQRT((C12/B12)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S12</f>
-        <v>6.8217960029032368E-2</v>
+        <v>4.3112964975747143</v>
       </c>
       <c r="U12">
         <f t="shared" si="4"/>
-        <v>1346.7771506366844</v>
+        <v>3013.7290078798574</v>
       </c>
       <c r="W12">
         <f t="shared" si="5"/>
-        <v>0.87500624747933731</v>
+        <v>0.93999411718729731</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -7392,19 +7392,19 @@
       </c>
       <c r="S13">
         <f>B13*Parameters!$B$6</f>
-        <v>46.944468354083234</v>
+        <v>97.786500000000004</v>
       </c>
       <c r="T13">
         <f>SQRT((C13/B13)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S13</f>
-        <v>6.8217960029032368E-2</v>
+        <v>4.3112964975747143</v>
       </c>
       <c r="U13">
         <f t="shared" si="4"/>
-        <v>1380.165850772047</v>
+        <v>3080.568246956554</v>
       </c>
       <c r="W13">
         <f t="shared" si="5"/>
-        <v>0.87905903261752028</v>
+        <v>0.9419397420298401</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -7460,19 +7460,19 @@
       </c>
       <c r="S14">
         <f>B14*Parameters!$B$6</f>
-        <v>117.53003587928751</v>
+        <v>244.81799999999998</v>
       </c>
       <c r="T14">
         <f>SQRT((C14/B14)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S14</f>
-        <v>0.67588312473327705</v>
+        <v>10.879365468629134</v>
       </c>
       <c r="U14">
         <f t="shared" si="4"/>
-        <v>3219.6733463149226</v>
+        <v>7420.5962545892608</v>
       </c>
       <c r="W14">
         <f t="shared" si="5"/>
-        <v>0.83005251945587644</v>
+        <v>0.91841313348713993</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -7528,19 +7528,19 @@
       </c>
       <c r="S15">
         <f>B15*Parameters!$B$6</f>
-        <v>117.53003587928751</v>
+        <v>244.81799999999998</v>
       </c>
       <c r="T15">
         <f>SQRT((C15/B15)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S15</f>
-        <v>0.67588312473327705</v>
+        <v>10.879365468629134</v>
       </c>
       <c r="U15">
         <f t="shared" si="4"/>
-        <v>3041.5979438521617</v>
+        <v>7327.3879815865885</v>
       </c>
       <c r="W15">
         <f t="shared" si="5"/>
-        <v>0.76861593937732442</v>
+        <v>0.88891920958884441</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -7596,19 +7596,19 @@
       </c>
       <c r="S16">
         <f>B16*Parameters!$B$6</f>
-        <v>117.53003587928751</v>
+        <v>244.81799999999998</v>
       </c>
       <c r="T16">
         <f>SQRT((C16/B16)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S16</f>
-        <v>0.67588312473327705</v>
+        <v>10.879365468629134</v>
       </c>
       <c r="U16">
         <f t="shared" si="4"/>
-        <v>3047.1943075101044</v>
+        <v>7248.117215784443</v>
       </c>
       <c r="W16">
         <f t="shared" si="5"/>
-        <v>0.78558631269700485</v>
+        <v>0.89706619463547876</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -7660,19 +7660,19 @@
       </c>
       <c r="S17">
         <f>B17*Parameters!$B$6</f>
-        <v>235.06007175857502</v>
+        <v>489.63599999999997</v>
       </c>
       <c r="T17">
         <f>SQRT((C17/B17)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S17</f>
-        <v>0.67715098344118985</v>
+        <v>21.621827512955516</v>
       </c>
       <c r="U17">
         <f t="shared" si="4"/>
-        <v>6173.378466917482</v>
+        <v>14547.58663275383</v>
       </c>
       <c r="W17">
         <f t="shared" si="5"/>
-        <v>0.79839465712000568</v>
+        <v>0.90321511007302657</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -7724,19 +7724,19 @@
       </c>
       <c r="S18">
         <f>B18*Parameters!$B$6</f>
-        <v>235.06007175857502</v>
+        <v>489.63599999999997</v>
       </c>
       <c r="T18">
         <f>SQRT((C18/B18)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S18</f>
-        <v>0.67715098344118985</v>
+        <v>21.621827512955516</v>
       </c>
       <c r="U18">
         <f t="shared" si="4"/>
-        <v>6293.9073662439405</v>
+        <v>14808.152457930393</v>
       </c>
       <c r="W18">
         <f t="shared" si="5"/>
-        <v>0.80059462605787579</v>
+        <v>0.90427125148501908</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
@@ -7788,19 +7788,19 @@
       </c>
       <c r="S19">
         <f>B19*Parameters!$B$6</f>
-        <v>235.06007175857502</v>
+        <v>489.63599999999997</v>
       </c>
       <c r="T19">
         <f>SQRT((C19/B19)^2+(Parameters!$C$6/Parameters!$B$6)^2)*'Bottle Results'!S19</f>
-        <v>0.67715098344118985</v>
+        <v>21.621827512955516</v>
       </c>
       <c r="U19">
         <f t="shared" si="4"/>
-        <v>6141.3105900445398</v>
+        <v>14684.126973984974</v>
       </c>
       <c r="W19">
         <f t="shared" si="5"/>
-        <v>0.77857142735536078</v>
+        <v>0.89369855121917563</v>
       </c>
     </row>
   </sheetData>
@@ -7812,8 +7812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7901,23 +7901,23 @@
       </c>
       <c r="D3">
         <f>AVERAGE('Bottle Results'!U5:U7)</f>
-        <v>103.54252794844137</v>
+        <v>270.81622261908865</v>
       </c>
       <c r="E3">
         <f>_xlfn.STDEV.S('Bottle Results'!U5:U7)</f>
-        <v>0.77420866487608486</v>
+        <v>3.5223545816029764</v>
       </c>
       <c r="F3">
         <f>AVERAGE('Bottle Results'!S5:S7)</f>
-        <v>4.6944468354083231</v>
+        <v>9.778649999999999</v>
       </c>
       <c r="G3">
         <f>AVERAGE('Bottle Results'!W5:W7)</f>
-        <v>0.67045950904498197</v>
+        <v>0.84179714838932884</v>
       </c>
       <c r="H3">
         <f>_xlfn.STDEV.S('Bottle Results'!W5:W7)</f>
-        <v>6.0774582078356437E-3</v>
+        <v>2.9176117819023442E-3</v>
       </c>
       <c r="I3">
         <f>AVERAGE('Bottle Results'!D5:D7)</f>
@@ -7942,23 +7942,23 @@
       </c>
       <c r="D4">
         <f>AVERAGE('Bottle Results'!U8:U10)</f>
-        <v>693.17438610025908</v>
+        <v>1543.9279231594101</v>
       </c>
       <c r="E4">
         <f>_xlfn.STDEV.S('Bottle Results'!U8:U10)</f>
-        <v>10.218939358344871</v>
+        <v>27.390610686569982</v>
       </c>
       <c r="F4">
         <f>AVERAGE('Bottle Results'!S8:S10)</f>
-        <v>23.506007175857501</v>
+        <v>48.963600000000007</v>
       </c>
       <c r="G4">
         <f>AVERAGE('Bottle Results'!W8:W10)</f>
-        <v>0.88256124174599648</v>
+        <v>0.94362105126578921</v>
       </c>
       <c r="H4">
         <f>_xlfn.STDEV.S('Bottle Results'!W8:W10)</f>
-        <v>1.2380080330185188E-2</v>
+        <v>5.9433182421027844E-3</v>
       </c>
       <c r="I4">
         <f>AVERAGE('Bottle Results'!D8:D10)</f>
@@ -7983,23 +7983,23 @@
       </c>
       <c r="D5">
         <f>AVERAGE('Bottle Results'!U11:U13)</f>
-        <v>1343.2746297137428</v>
+        <v>3025.0443274560475</v>
       </c>
       <c r="E5">
         <f>_xlfn.STDEV.S('Bottle Results'!U11:U13)</f>
-        <v>38.761348243035506</v>
+        <v>50.819988198928094</v>
       </c>
       <c r="F5">
         <f>AVERAGE('Bottle Results'!S11:S13)</f>
-        <v>46.944468354083234</v>
+        <v>97.786500000000004</v>
       </c>
       <c r="G5">
         <f>AVERAGE('Bottle Results'!W11:W13)</f>
-        <v>0.86500040865270356</v>
+        <v>0.93519060357189066</v>
       </c>
       <c r="H5">
         <f>_xlfn.STDEV.S('Bottle Results'!W11:W13)</f>
-        <v>2.0938721162594591E-2</v>
+        <v>1.0052073987640393E-2</v>
       </c>
       <c r="I5">
         <f>AVERAGE('Bottle Results'!D11:D13)</f>
@@ -8024,23 +8024,23 @@
       </c>
       <c r="D6">
         <f>AVERAGE('Bottle Results'!U14:U16)</f>
-        <v>3102.8218658923961</v>
+        <v>7332.0338173200971</v>
       </c>
       <c r="E6">
         <f>_xlfn.STDEV.S('Bottle Results'!U14:U16)</f>
-        <v>101.23502940805632</v>
+        <v>86.333322355887105</v>
       </c>
       <c r="F6">
         <f>AVERAGE('Bottle Results'!S14:S16)</f>
-        <v>117.5300358792875</v>
+        <v>244.81799999999998</v>
       </c>
       <c r="G6">
         <f>AVERAGE('Bottle Results'!W14:W16)</f>
-        <v>0.7947515905100685</v>
+        <v>0.90146617923715444</v>
       </c>
       <c r="H6">
         <f>_xlfn.STDEV.S('Bottle Results'!W14:W16)</f>
-        <v>3.1727197811657781E-2</v>
+        <v>1.5231309369218682E-2</v>
       </c>
       <c r="I6">
         <f>AVERAGE('Bottle Results'!D14:D16)</f>
@@ -8065,23 +8065,23 @@
       </c>
       <c r="D7">
         <f>AVERAGE('Bottle Results'!U17:U19)</f>
-        <v>6202.8654744019877</v>
+        <v>14679.955354889733</v>
       </c>
       <c r="E7">
         <f>_xlfn.STDEV.S('Bottle Results'!U17:U19)</f>
-        <v>80.458416181316622</v>
+        <v>130.33299320161686</v>
       </c>
       <c r="F7">
         <f>AVERAGE('Bottle Results'!S17:S19)</f>
-        <v>235.06007175857499</v>
+        <v>489.63599999999997</v>
       </c>
       <c r="G7">
         <f>AVERAGE('Bottle Results'!W17:W19)</f>
-        <v>0.79252023684441408</v>
+        <v>0.9003949709257405</v>
       </c>
       <c r="H7">
         <f>_xlfn.STDEV.S('Bottle Results'!W17:W19)</f>
-        <v>1.2130001255289546E-2</v>
+        <v>5.8232625164407106E-3</v>
       </c>
       <c r="I7">
         <f>AVERAGE('Bottle Results'!D17:D19)</f>

</xml_diff>